<commit_message>
colocando todos os tipos de bancos possiveis
</commit_message>
<xml_diff>
--- a/ubsWP/bd/tabela_endereco.xlsx
+++ b/ubsWP/bd/tabela_endereco.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="550">
   <si>
     <t>endereco</t>
   </si>
@@ -612,1064 +612,1061 @@
     <t>SHLN 516 cj D  - Asa Norte</t>
   </si>
   <si>
-    <t>SHIS QI 15 Área Especial</t>
-  </si>
-  <si>
-    <t>Área Especial nº 6, Setor tradicional - Brazlândia</t>
-  </si>
-  <si>
     <t>SMHS Quadra 301 Bloco A - Asa Sul</t>
   </si>
   <si>
     <t>SHLS 716 Conjunto E - Asa Sul</t>
   </si>
   <si>
-    <t>SHIS, QI 07, Conjunto F</t>
-  </si>
-  <si>
     <t>Av. L2 Sul Quadra 608, Módulo A</t>
   </si>
   <si>
-    <t>SMHN 101 Área Especial - Asa Norte</t>
-  </si>
-  <si>
     <t>SAAN Quadra 1 Lote 25/35 - Asa Norte</t>
   </si>
   <si>
-    <t>Setor E, Área Especial 01 e 17, Taguatinga Sul</t>
-  </si>
-  <si>
     <t>Smu Hgub, bl Sn</t>
   </si>
   <si>
     <t>SEPS 711/911, s/n bl A</t>
   </si>
   <si>
-    <t>Quadra 12 - Área Especial - Setor Central_x000D_
+    <t xml:space="preserve"> Estrada Contorno do Bosque, Cruzeiro Novo</t>
+  </si>
+  <si>
+    <t>Sgas 613, Conjunto C, Asa Sul</t>
+  </si>
+  <si>
+    <t>R. SGAN 608 Md F - Asa norte</t>
+  </si>
+  <si>
+    <t>Sain Lt 04 - Srpn</t>
+  </si>
+  <si>
+    <t>Lt 04, Shcnw Trecho 2 - SRPN</t>
+  </si>
+  <si>
+    <t>Riacho Fundo I Ac 4 Qn 9</t>
+  </si>
+  <si>
+    <t>Riacho Fundo II-1A Etapa Qn 7B Conjunto 3</t>
+  </si>
+  <si>
+    <t>Quadra 102 Conjunto 1 Lote 1</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>-47.6473617553697</t>
+  </si>
+  <si>
+    <t>-15.6389522552486</t>
+  </si>
+  <si>
+    <t>-48.0602717399583</t>
+  </si>
+  <si>
+    <t>-15.9021949768062</t>
+  </si>
+  <si>
+    <t>-47.6433491706834</t>
+  </si>
+  <si>
+    <t>-15.6122589111324</t>
+  </si>
+  <si>
+    <t>-48.1050109863267</t>
+  </si>
+  <si>
+    <t>-15.8355689048762</t>
+  </si>
+  <si>
+    <t>-47.8740835189805</t>
+  </si>
+  <si>
+    <t>-15.7255876064296</t>
+  </si>
+  <si>
+    <t>-47.892365455626</t>
+  </si>
+  <si>
+    <t>-15.7734704017635</t>
+  </si>
+  <si>
+    <t>-48.0473542213426</t>
+  </si>
+  <si>
+    <t>-15.8512651920314</t>
+  </si>
+  <si>
+    <t>-47.7775454521165</t>
+  </si>
+  <si>
+    <t>-15.9076666831966</t>
+  </si>
+  <si>
+    <t>-47.5177145004259</t>
+  </si>
+  <si>
+    <t>-15.9070014953609</t>
+  </si>
+  <si>
+    <t>-47.9703211784349</t>
+  </si>
+  <si>
+    <t>-15.8489906787868</t>
+  </si>
+  <si>
+    <t>-47.493059635161</t>
+  </si>
+  <si>
+    <t>-15.7626235485072</t>
+  </si>
+  <si>
+    <t>-47.5109553337083</t>
+  </si>
+  <si>
+    <t>-15.5343568325038</t>
+  </si>
+  <si>
+    <t>-47.670278549193</t>
+  </si>
+  <si>
+    <t>-15.6353259086604</t>
+  </si>
+  <si>
+    <t>-47.8378629684434</t>
+  </si>
+  <si>
+    <t>-15.6340706348415</t>
+  </si>
+  <si>
+    <t>-47.9998683929429</t>
+  </si>
+  <si>
+    <t>-15.7802188396449</t>
+  </si>
+  <si>
+    <t>-48.1102466583238</t>
+  </si>
+  <si>
+    <t>-15.8758127689357</t>
+  </si>
+  <si>
+    <t>-47.9352378845201</t>
+  </si>
+  <si>
+    <t>-15.563560724258</t>
+  </si>
+  <si>
+    <t>-48.0791759490953</t>
+  </si>
+  <si>
+    <t>-15.8626055717464</t>
+  </si>
+  <si>
+    <t>-47.8762292861925</t>
+  </si>
+  <si>
+    <t>-15.710706710815</t>
+  </si>
+  <si>
+    <t>-47.9887318611131</t>
+  </si>
+  <si>
+    <t>-15.8104312419887</t>
+  </si>
+  <si>
+    <t>-47.7722668647752</t>
+  </si>
+  <si>
+    <t>-15.9040081501002</t>
+  </si>
+  <si>
+    <t>-48.1990170478807</t>
+  </si>
+  <si>
+    <t>-15.6744217872615</t>
+  </si>
+  <si>
+    <t>-47.557003498076</t>
+  </si>
+  <si>
+    <t>-15.9630489349361</t>
+  </si>
+  <si>
+    <t>-48.1335496902452</t>
+  </si>
+  <si>
+    <t>-15.7983720302577</t>
+  </si>
+  <si>
+    <t>-48.1948328018174</t>
+  </si>
+  <si>
+    <t>-15.6770718097682</t>
+  </si>
+  <si>
+    <t>-48.2359457015977</t>
+  </si>
+  <si>
+    <t>-15.9419775009151</t>
+  </si>
+  <si>
+    <t>-47.7776527404771</t>
+  </si>
+  <si>
+    <t>-15.8900606632228</t>
+  </si>
+  <si>
+    <t>-48.1117057800279</t>
+  </si>
+  <si>
+    <t>-15.8031249046321</t>
+  </si>
+  <si>
+    <t>-47.6483917236314</t>
+  </si>
+  <si>
+    <t>-15.6793248653407</t>
+  </si>
+  <si>
+    <t>-47.8804993629442</t>
+  </si>
+  <si>
+    <t>-15.761497020721</t>
+  </si>
+  <si>
+    <t>-47.6525330543504</t>
+  </si>
+  <si>
+    <t>-15.6774258613582</t>
+  </si>
+  <si>
+    <t>-47.7696919441209</t>
+  </si>
+  <si>
+    <t>-15.7454466819759</t>
+  </si>
+  <si>
+    <t>-47.7532982826219</t>
+  </si>
+  <si>
+    <t>-15.9091258049007</t>
+  </si>
+  <si>
+    <t>-47.8914213180528</t>
+  </si>
+  <si>
+    <t>-15.7430434226985</t>
+  </si>
+  <si>
+    <t>-47.5693845748888</t>
+  </si>
+  <si>
+    <t>-15.8205592632289</t>
+  </si>
+  <si>
+    <t>-47.7799057960496</t>
+  </si>
+  <si>
+    <t>-15.7696187496181</t>
+  </si>
+  <si>
+    <t>-47.7532553672777</t>
+  </si>
+  <si>
+    <t>-15.9093296527858</t>
+  </si>
+  <si>
+    <t>-48.1703066825853</t>
+  </si>
+  <si>
+    <t>-15.7429790496822</t>
+  </si>
+  <si>
+    <t>-47.9482841491685</t>
+  </si>
+  <si>
+    <t>-15.6190824508662</t>
+  </si>
+  <si>
+    <t>-48.0599713325486</t>
+  </si>
+  <si>
+    <t>-15.9021520614619</t>
+  </si>
+  <si>
+    <t>-48.2464814186082</t>
+  </si>
+  <si>
+    <t>-15.8289062976833</t>
+  </si>
+  <si>
+    <t>-48.1206536293016</t>
+  </si>
+  <si>
+    <t>-15.8078455924983</t>
+  </si>
+  <si>
+    <t>-48.0685973167405</t>
+  </si>
+  <si>
+    <t>-15.8784091472621</t>
+  </si>
+  <si>
+    <t>-48.06130170822</t>
+  </si>
+  <si>
+    <t>-16.036520004272</t>
+  </si>
+  <si>
+    <t>-47.6402807235704</t>
+  </si>
+  <si>
+    <t>-15.6407654285426</t>
+  </si>
+  <si>
+    <t>-47.93</t>
+  </si>
+  <si>
+    <t>-15.78</t>
+  </si>
+  <si>
+    <t>-48.0632328987108</t>
+  </si>
+  <si>
+    <t>-15.8105170726772</t>
+  </si>
+  <si>
+    <t>-48.0010056495653</t>
+  </si>
+  <si>
+    <t>-15.879642963409</t>
+  </si>
+  <si>
+    <t>-15.8079314231868</t>
+  </si>
+  <si>
+    <t>-48.0526328086839</t>
+  </si>
+  <si>
+    <t>-16.0057604312892</t>
+  </si>
+  <si>
+    <t>-48.1435489654527</t>
+  </si>
+  <si>
+    <t>-15.8047878742213</t>
+  </si>
+  <si>
+    <t>-47.8215980529771</t>
+  </si>
+  <si>
+    <t>-15.621024370193</t>
+  </si>
+  <si>
+    <t>-48.1144094467149</t>
+  </si>
+  <si>
+    <t>-15.8400750160213</t>
+  </si>
+  <si>
+    <t>-47.9731106758104</t>
+  </si>
+  <si>
+    <t>-15.8327364921565</t>
+  </si>
+  <si>
+    <t>-48.199081420897</t>
+  </si>
+  <si>
+    <t>-15.6693577766414</t>
+  </si>
+  <si>
+    <t>-47.6625108718858</t>
+  </si>
+  <si>
+    <t>-15.7465732097621</t>
+  </si>
+  <si>
+    <t>-47.7606368064867</t>
+  </si>
+  <si>
+    <t>-15.914597511291</t>
+  </si>
+  <si>
+    <t>-48.1056547164903</t>
+  </si>
+  <si>
+    <t>-15.9301865100856</t>
+  </si>
+  <si>
+    <t>-48.0442428588853</t>
+  </si>
+  <si>
+    <t>-16.0458755493159</t>
+  </si>
+  <si>
+    <t>-47.9240155220018</t>
+  </si>
+  <si>
+    <t>-15.8254301548</t>
+  </si>
+  <si>
+    <t>-47.8134870529161</t>
+  </si>
+  <si>
+    <t>-15.9908902645106</t>
+  </si>
+  <si>
+    <t>-47.9358386993394</t>
+  </si>
+  <si>
+    <t>-15.783298015594</t>
+  </si>
+  <si>
+    <t>-48.1016635894761</t>
+  </si>
+  <si>
+    <t>-15.9196507930751</t>
+  </si>
+  <si>
+    <t>-48.0925440788255</t>
+  </si>
+  <si>
+    <t>-15.8210635185237</t>
+  </si>
+  <si>
+    <t>-47.3735404014574</t>
+  </si>
+  <si>
+    <t>-15.7040226459499</t>
+  </si>
+  <si>
+    <t>-47.7632975578294</t>
+  </si>
+  <si>
+    <t>-15.7402324676509</t>
+  </si>
+  <si>
+    <t>-48.067417144774</t>
+  </si>
+  <si>
+    <t>-16.0136997699733</t>
+  </si>
+  <si>
+    <t>-47.8716588020311</t>
+  </si>
+  <si>
+    <t>-15.6003499031062</t>
+  </si>
+  <si>
+    <t>-47.9514169692979</t>
+  </si>
+  <si>
+    <t>-15.8500099182124</t>
+  </si>
+  <si>
+    <t>-47.9396367073045</t>
+  </si>
+  <si>
+    <t>-15.9336304664607</t>
+  </si>
+  <si>
+    <t>-47.7819657325731</t>
+  </si>
+  <si>
+    <t>-15.6504642963405</t>
+  </si>
+  <si>
+    <t>-47.9096817970262</t>
+  </si>
+  <si>
+    <t>-15.8326828479762</t>
+  </si>
+  <si>
+    <t>-48.0741977691636</t>
+  </si>
+  <si>
+    <t>-16.0116505622859</t>
+  </si>
+  <si>
+    <t>-47.6482844352708</t>
+  </si>
+  <si>
+    <t>-15.6028389930721</t>
+  </si>
+  <si>
+    <t>-48.0870294570909</t>
+  </si>
+  <si>
+    <t>-15.88415980339</t>
+  </si>
+  <si>
+    <t>-48.0997538566575</t>
+  </si>
+  <si>
+    <t>-15.9644651412959</t>
+  </si>
+  <si>
+    <t>-48.0024218559251</t>
+  </si>
+  <si>
+    <t>-16.0103952884669</t>
+  </si>
+  <si>
+    <t>-47.5556516647325</t>
+  </si>
+  <si>
+    <t>-16.0085391998286</t>
+  </si>
+  <si>
+    <t>-47.3805141448961</t>
+  </si>
+  <si>
+    <t>-16.016532182693</t>
+  </si>
+  <si>
+    <t>-47.9972720146165</t>
+  </si>
+  <si>
+    <t>-15.7834482192989</t>
+  </si>
+  <si>
+    <t>-48.0630397796617</t>
+  </si>
+  <si>
+    <t>-15.8364593982692</t>
+  </si>
+  <si>
+    <t>-48.059670925139</t>
+  </si>
+  <si>
+    <t>-15.795539617538</t>
+  </si>
+  <si>
+    <t>-47.9864573478685</t>
+  </si>
+  <si>
+    <t>-15.8183705806728</t>
+  </si>
+  <si>
+    <t>-47.8892111778245</t>
+  </si>
+  <si>
+    <t>-15.6459367275233</t>
+  </si>
+  <si>
+    <t>-47.9881095886217</t>
+  </si>
+  <si>
+    <t>-15.9931969642635</t>
+  </si>
+  <si>
+    <t>-47.6515674591051</t>
+  </si>
+  <si>
+    <t>-15.6247580051418</t>
+  </si>
+  <si>
+    <t>-48.0149316787706</t>
+  </si>
+  <si>
+    <t>-15.9475350379939</t>
+  </si>
+  <si>
+    <t>-47.6802349090562</t>
+  </si>
+  <si>
+    <t>-15.6201660633083</t>
+  </si>
+  <si>
+    <t>-47.793123722075</t>
+  </si>
+  <si>
+    <t>-15.876585245132</t>
+  </si>
+  <si>
+    <t>-47.9135441780076</t>
+  </si>
+  <si>
+    <t>-15.7087004184718</t>
+  </si>
+  <si>
+    <t>-48.0458307266221</t>
+  </si>
+  <si>
+    <t>-15.905767679214</t>
+  </si>
+  <si>
+    <t>-47.5213623046861</t>
+  </si>
+  <si>
+    <t>-15.6333196163173</t>
+  </si>
+  <si>
+    <t>-48.1365966796861</t>
+  </si>
+  <si>
+    <t>-15.7851541042323</t>
+  </si>
+  <si>
+    <t>-48.1686115264879</t>
+  </si>
+  <si>
+    <t>-15.5390453338619</t>
+  </si>
+  <si>
+    <t>-48.0721378326402</t>
+  </si>
+  <si>
+    <t>-15.980322360992</t>
+  </si>
+  <si>
+    <t>-47.9656219482408</t>
+  </si>
+  <si>
+    <t>-15.8703088760371</t>
+  </si>
+  <si>
+    <t>-48.0675458908067</t>
+  </si>
+  <si>
+    <t>-15.8229839801784</t>
+  </si>
+  <si>
+    <t>-47.8480339050279</t>
+  </si>
+  <si>
+    <t>-15.7951962947841</t>
+  </si>
+  <si>
+    <t>-48.2544851303087</t>
+  </si>
+  <si>
+    <t>-16.0436546802516</t>
+  </si>
+  <si>
+    <t>-48.1253743171678</t>
+  </si>
+  <si>
+    <t>-15.967179536819</t>
+  </si>
+  <si>
+    <t>-48.049221038817</t>
+  </si>
+  <si>
+    <t>-15.9094369411464</t>
+  </si>
+  <si>
+    <t>-47.8094744682298</t>
+  </si>
+  <si>
+    <t>-15.6548202037807</t>
+  </si>
+  <si>
+    <t>-47.8243660926805</t>
+  </si>
+  <si>
+    <t>-15.6446492671962</t>
+  </si>
+  <si>
+    <t>-48.0939602851854</t>
+  </si>
+  <si>
+    <t>-15.8012902736659</t>
+  </si>
+  <si>
+    <t>-48.0437493324266</t>
+  </si>
+  <si>
+    <t>-15.9012722969051</t>
+  </si>
+  <si>
+    <t>-48.0437922477708</t>
+  </si>
+  <si>
+    <t>-15.9227192401881</t>
+  </si>
+  <si>
+    <t>-48.0677175521837</t>
+  </si>
+  <si>
+    <t>-16.0134530067439</t>
+  </si>
+  <si>
+    <t>-48.142154216765</t>
+  </si>
+  <si>
+    <t>-15.890103578567</t>
+  </si>
+  <si>
+    <t>-48.0263257026658</t>
+  </si>
+  <si>
+    <t>-16.027153730392</t>
+  </si>
+  <si>
+    <t>-47.9421901702867</t>
+  </si>
+  <si>
+    <t>-15.8008074760432</t>
+  </si>
+  <si>
+    <t>-47.8549861907945</t>
+  </si>
+  <si>
+    <t>-15.846877098083</t>
+  </si>
+  <si>
+    <t>-48.1980943679796</t>
+  </si>
+  <si>
+    <t>-15.6651949882503</t>
+  </si>
+  <si>
+    <t>-48.1298375129686</t>
+  </si>
+  <si>
+    <t>-15.8069336414333</t>
+  </si>
+  <si>
+    <t>-47.618780136107</t>
+  </si>
+  <si>
+    <t>-15.5236172676082</t>
+  </si>
+  <si>
+    <t>-47.7717304229722</t>
+  </si>
+  <si>
+    <t>-15.916571617126</t>
+  </si>
+  <si>
+    <t>-47.7611732482896</t>
+  </si>
+  <si>
+    <t>-15.8979463577266</t>
+  </si>
+  <si>
+    <t>-47.7880382537828</t>
+  </si>
+  <si>
+    <t>-15.8955860137935</t>
+  </si>
+  <si>
+    <t>-47.7558517456041</t>
+  </si>
+  <si>
+    <t>-15.9051239490504</t>
+  </si>
+  <si>
+    <t>-48.0239224433885</t>
+  </si>
+  <si>
+    <t>-15.8856081962581</t>
+  </si>
+  <si>
+    <t>-48.0239868164049</t>
+  </si>
+  <si>
+    <t>-15.8595371246333</t>
+  </si>
+  <si>
+    <t>-48.0566239356981</t>
+  </si>
+  <si>
+    <t>-16.0253727436061</t>
+  </si>
+  <si>
+    <t>-47.6578116416917</t>
+  </si>
+  <si>
+    <t>-15.6149840354915</t>
+  </si>
+  <si>
+    <t>-47.9895901679979</t>
+  </si>
+  <si>
+    <t>-16.0073912143703</t>
+  </si>
+  <si>
+    <t>-48.1309747695909</t>
+  </si>
+  <si>
+    <t>-15.7956469058986</t>
+  </si>
+  <si>
+    <t>-48.0963635444627</t>
+  </si>
+  <si>
+    <t>-15.8309447765346</t>
+  </si>
+  <si>
+    <t>-47.7785968780504</t>
+  </si>
+  <si>
+    <t>-15.7706701755519</t>
+  </si>
+  <si>
+    <t>-48.200690746306</t>
+  </si>
+  <si>
+    <t>-15.6698405742641</t>
+  </si>
+  <si>
+    <t>-47.8468751907335</t>
+  </si>
+  <si>
+    <t>-15.6358623504634</t>
+  </si>
+  <si>
+    <t>-48.1121778488145</t>
+  </si>
+  <si>
+    <t>-15.8906614780421</t>
+  </si>
+  <si>
+    <t>-48.0734467506395</t>
+  </si>
+  <si>
+    <t>-16.0115647315974</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>-15.800896</t>
+  </si>
+  <si>
+    <t>-15.813201</t>
+  </si>
+  <si>
+    <t>-15.735378</t>
+  </si>
+  <si>
+    <t>-15.828578</t>
+  </si>
+  <si>
+    <t>-15.735693</t>
+  </si>
+  <si>
+    <t>-15.845447</t>
+  </si>
+  <si>
+    <t>-15.675074</t>
+  </si>
+  <si>
+    <t>-15.798894</t>
+  </si>
+  <si>
+    <t>-15.827313</t>
+  </si>
+  <si>
+    <t>-15.841474</t>
+  </si>
+  <si>
+    <t>-15.821942</t>
+  </si>
+  <si>
+    <t>-15.785673</t>
+  </si>
+  <si>
+    <t>-15.815309</t>
+  </si>
+  <si>
+    <t>-15.859855</t>
+  </si>
+  <si>
+    <t>-15.772759</t>
+  </si>
+  <si>
+    <t>-15.814717</t>
+  </si>
+  <si>
+    <t>-15.648612</t>
+  </si>
+  <si>
+    <t>-15.801392</t>
+  </si>
+  <si>
+    <t>-15.820160</t>
+  </si>
+  <si>
+    <t>-15.759256</t>
+  </si>
+  <si>
+    <t>-15.885181</t>
+  </si>
+  <si>
+    <t>-15.833847</t>
+  </si>
+  <si>
+    <t>-15.760302</t>
+  </si>
+  <si>
+    <t>-15.759768</t>
+  </si>
+  <si>
+    <t>-15.823967</t>
+  </si>
+  <si>
+    <t>-15.870194</t>
+  </si>
+  <si>
+    <t>-15.905819</t>
+  </si>
+  <si>
+    <t>-15.817710</t>
+  </si>
+  <si>
+    <t>-15.911784</t>
+  </si>
+  <si>
+    <t>-15.900793</t>
+  </si>
+  <si>
+    <t>-15.883017</t>
+  </si>
+  <si>
+    <t>-15.875977</t>
+  </si>
+  <si>
+    <t>-47.982235</t>
+  </si>
+  <si>
+    <t>-48.099695</t>
+  </si>
+  <si>
+    <t>-47.777748</t>
+  </si>
+  <si>
+    <t>-48.057594</t>
+  </si>
+  <si>
+    <t>-47.986099</t>
+  </si>
+  <si>
+    <t>-48.046297</t>
+  </si>
+  <si>
+    <t>-48.023552</t>
+  </si>
+  <si>
+    <t>-47.965691</t>
+  </si>
+  <si>
+    <t>-47.888969</t>
+  </si>
+  <si>
+    <t>-47.912131</t>
+  </si>
+  <si>
+    <t>-47.895309</t>
+  </si>
+  <si>
+    <t>-47.929166</t>
+  </si>
+  <si>
+    <t>-47.897239</t>
+  </si>
+  <si>
+    <t>-47.882990</t>
+  </si>
+  <si>
+    <t>-48.203996</t>
+  </si>
+  <si>
+    <t>-47.890001</t>
+  </si>
+  <si>
+    <t>-47.930522</t>
+  </si>
+  <si>
+    <t>-47.885285</t>
+  </si>
+  <si>
+    <t>-47.896106</t>
+  </si>
+  <si>
+    <t>-47.882863</t>
+  </si>
+  <si>
+    <t>-47.908292</t>
+  </si>
+  <si>
+    <t>-48.042606</t>
+  </si>
+  <si>
+    <t>-47.930484</t>
+  </si>
+  <si>
+    <t>-47.914739</t>
+  </si>
+  <si>
+    <t>-47.792290</t>
+  </si>
+  <si>
+    <t>-47.936691</t>
+  </si>
+  <si>
+    <t>-47.926535</t>
+  </si>
+  <si>
+    <t>-47.911386</t>
+  </si>
+  <si>
+    <t>-47.876796</t>
+  </si>
+  <si>
+    <t>-47.915299</t>
+  </si>
+  <si>
+    <t>-47.917464</t>
+  </si>
+  <si>
+    <t>-48.066628</t>
+  </si>
+  <si>
+    <t>SHIS QI 15 Area Especial</t>
+  </si>
+  <si>
+    <t>SMHN 101 Area Especial - Asa Norte</t>
+  </si>
+  <si>
+    <t>Setor E, Area Especial 01 e 17, Taguatinga Sul</t>
+  </si>
+  <si>
+    <t>Quadra 12 - Area Especial - Setor Central_x000D_
  Sobradinho</t>
   </si>
   <si>
-    <t xml:space="preserve"> Estrada Contorno do Bosque, Cruzeiro Novo</t>
-  </si>
-  <si>
-    <t>Setor de Grandes Áreas Sul 915</t>
-  </si>
-  <si>
-    <t>Sgas 613, Conjunto C, Asa Sul</t>
-  </si>
-  <si>
-    <t>R. SGAN 608 Md F - Asa norte</t>
-  </si>
-  <si>
-    <t>Sain Lt 04 - Srpn</t>
-  </si>
-  <si>
-    <t>Lt 04, Shcnw Trecho 2 - SRPN</t>
-  </si>
-  <si>
-    <t>Área Especial 8, ae 8/9 sl 118 B</t>
-  </si>
-  <si>
-    <t>Área Especial 03, 3ª Avenida - Núcleo Bandeirante</t>
-  </si>
-  <si>
-    <t>Riacho Fundo I Ac 4 Qn 9</t>
-  </si>
-  <si>
-    <t>Riacho Fundo II-1A Etapa Qn 7B Conjunto 3</t>
-  </si>
-  <si>
-    <t>Área Especial – QI O6 Lote C – Guará I</t>
-  </si>
-  <si>
-    <t>Quadra 400/600 Área Especial</t>
-  </si>
-  <si>
-    <t>Quadra 102 Conjunto 1 Lote 1</t>
-  </si>
-  <si>
-    <t>QS 107 Conjunto 4 Área Especial</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DF-075, KM 180, Área Especial EPNB</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>-47.6473617553697</t>
-  </si>
-  <si>
-    <t>-15.6389522552486</t>
-  </si>
-  <si>
-    <t>-48.0602717399583</t>
-  </si>
-  <si>
-    <t>-15.9021949768062</t>
-  </si>
-  <si>
-    <t>-47.6433491706834</t>
-  </si>
-  <si>
-    <t>-15.6122589111324</t>
-  </si>
-  <si>
-    <t>-48.1050109863267</t>
-  </si>
-  <si>
-    <t>-15.8355689048762</t>
-  </si>
-  <si>
-    <t>-47.8740835189805</t>
-  </si>
-  <si>
-    <t>-15.7255876064296</t>
-  </si>
-  <si>
-    <t>-47.892365455626</t>
-  </si>
-  <si>
-    <t>-15.7734704017635</t>
-  </si>
-  <si>
-    <t>-48.0473542213426</t>
-  </si>
-  <si>
-    <t>-15.8512651920314</t>
-  </si>
-  <si>
-    <t>-47.7775454521165</t>
-  </si>
-  <si>
-    <t>-15.9076666831966</t>
-  </si>
-  <si>
-    <t>-47.5177145004259</t>
-  </si>
-  <si>
-    <t>-15.9070014953609</t>
-  </si>
-  <si>
-    <t>-47.9703211784349</t>
-  </si>
-  <si>
-    <t>-15.8489906787868</t>
-  </si>
-  <si>
-    <t>-47.493059635161</t>
-  </si>
-  <si>
-    <t>-15.7626235485072</t>
-  </si>
-  <si>
-    <t>-47.5109553337083</t>
-  </si>
-  <si>
-    <t>-15.5343568325038</t>
-  </si>
-  <si>
-    <t>-47.670278549193</t>
-  </si>
-  <si>
-    <t>-15.6353259086604</t>
-  </si>
-  <si>
-    <t>-47.8378629684434</t>
-  </si>
-  <si>
-    <t>-15.6340706348415</t>
-  </si>
-  <si>
-    <t>-47.9998683929429</t>
-  </si>
-  <si>
-    <t>-15.7802188396449</t>
-  </si>
-  <si>
-    <t>-48.1102466583238</t>
-  </si>
-  <si>
-    <t>-15.8758127689357</t>
-  </si>
-  <si>
-    <t>-47.9352378845201</t>
-  </si>
-  <si>
-    <t>-15.563560724258</t>
-  </si>
-  <si>
-    <t>-48.0791759490953</t>
-  </si>
-  <si>
-    <t>-15.8626055717464</t>
-  </si>
-  <si>
-    <t>-47.8762292861925</t>
-  </si>
-  <si>
-    <t>-15.710706710815</t>
-  </si>
-  <si>
-    <t>-47.9887318611131</t>
-  </si>
-  <si>
-    <t>-15.8104312419887</t>
-  </si>
-  <si>
-    <t>-47.7722668647752</t>
-  </si>
-  <si>
-    <t>-15.9040081501002</t>
-  </si>
-  <si>
-    <t>-48.1990170478807</t>
-  </si>
-  <si>
-    <t>-15.6744217872615</t>
-  </si>
-  <si>
-    <t>-47.557003498076</t>
-  </si>
-  <si>
-    <t>-15.9630489349361</t>
-  </si>
-  <si>
-    <t>-48.1335496902452</t>
-  </si>
-  <si>
-    <t>-15.7983720302577</t>
-  </si>
-  <si>
-    <t>-48.1948328018174</t>
-  </si>
-  <si>
-    <t>-15.6770718097682</t>
-  </si>
-  <si>
-    <t>-48.2359457015977</t>
-  </si>
-  <si>
-    <t>-15.9419775009151</t>
-  </si>
-  <si>
-    <t>-47.7776527404771</t>
-  </si>
-  <si>
-    <t>-15.8900606632228</t>
-  </si>
-  <si>
-    <t>-48.1117057800279</t>
-  </si>
-  <si>
-    <t>-15.8031249046321</t>
-  </si>
-  <si>
-    <t>-47.6483917236314</t>
-  </si>
-  <si>
-    <t>-15.6793248653407</t>
-  </si>
-  <si>
-    <t>-47.8804993629442</t>
-  </si>
-  <si>
-    <t>-15.761497020721</t>
-  </si>
-  <si>
-    <t>-47.6525330543504</t>
-  </si>
-  <si>
-    <t>-15.6774258613582</t>
-  </si>
-  <si>
-    <t>-47.7696919441209</t>
-  </si>
-  <si>
-    <t>-15.7454466819759</t>
-  </si>
-  <si>
-    <t>-47.7532982826219</t>
-  </si>
-  <si>
-    <t>-15.9091258049007</t>
-  </si>
-  <si>
-    <t>-47.8914213180528</t>
-  </si>
-  <si>
-    <t>-15.7430434226985</t>
-  </si>
-  <si>
-    <t>-47.5693845748888</t>
-  </si>
-  <si>
-    <t>-15.8205592632289</t>
-  </si>
-  <si>
-    <t>-47.7799057960496</t>
-  </si>
-  <si>
-    <t>-15.7696187496181</t>
-  </si>
-  <si>
-    <t>-47.7532553672777</t>
-  </si>
-  <si>
-    <t>-15.9093296527858</t>
-  </si>
-  <si>
-    <t>-48.1703066825853</t>
-  </si>
-  <si>
-    <t>-15.7429790496822</t>
-  </si>
-  <si>
-    <t>-47.9482841491685</t>
-  </si>
-  <si>
-    <t>-15.6190824508662</t>
-  </si>
-  <si>
-    <t>-48.0599713325486</t>
-  </si>
-  <si>
-    <t>-15.9021520614619</t>
-  </si>
-  <si>
-    <t>-48.2464814186082</t>
-  </si>
-  <si>
-    <t>-15.8289062976833</t>
-  </si>
-  <si>
-    <t>-48.1206536293016</t>
-  </si>
-  <si>
-    <t>-15.8078455924983</t>
-  </si>
-  <si>
-    <t>-48.0685973167405</t>
-  </si>
-  <si>
-    <t>-15.8784091472621</t>
-  </si>
-  <si>
-    <t>-48.06130170822</t>
-  </si>
-  <si>
-    <t>-16.036520004272</t>
-  </si>
-  <si>
-    <t>-47.6402807235704</t>
-  </si>
-  <si>
-    <t>-15.6407654285426</t>
-  </si>
-  <si>
-    <t>-47.93</t>
-  </si>
-  <si>
-    <t>-15.78</t>
-  </si>
-  <si>
-    <t>-48.0632328987108</t>
-  </si>
-  <si>
-    <t>-15.8105170726772</t>
-  </si>
-  <si>
-    <t>-48.0010056495653</t>
-  </si>
-  <si>
-    <t>-15.879642963409</t>
-  </si>
-  <si>
-    <t>-15.8079314231868</t>
-  </si>
-  <si>
-    <t>-48.0526328086839</t>
-  </si>
-  <si>
-    <t>-16.0057604312892</t>
-  </si>
-  <si>
-    <t>-48.1435489654527</t>
-  </si>
-  <si>
-    <t>-15.8047878742213</t>
-  </si>
-  <si>
-    <t>-47.8215980529771</t>
-  </si>
-  <si>
-    <t>-15.621024370193</t>
-  </si>
-  <si>
-    <t>-48.1144094467149</t>
-  </si>
-  <si>
-    <t>-15.8400750160213</t>
-  </si>
-  <si>
-    <t>-47.9731106758104</t>
-  </si>
-  <si>
-    <t>-15.8327364921565</t>
-  </si>
-  <si>
-    <t>-48.199081420897</t>
-  </si>
-  <si>
-    <t>-15.6693577766414</t>
-  </si>
-  <si>
-    <t>-47.6625108718858</t>
-  </si>
-  <si>
-    <t>-15.7465732097621</t>
-  </si>
-  <si>
-    <t>-47.7606368064867</t>
-  </si>
-  <si>
-    <t>-15.914597511291</t>
-  </si>
-  <si>
-    <t>-48.1056547164903</t>
-  </si>
-  <si>
-    <t>-15.9301865100856</t>
-  </si>
-  <si>
-    <t>-48.0442428588853</t>
-  </si>
-  <si>
-    <t>-16.0458755493159</t>
-  </si>
-  <si>
-    <t>-47.9240155220018</t>
-  </si>
-  <si>
-    <t>-15.8254301548</t>
-  </si>
-  <si>
-    <t>-47.8134870529161</t>
-  </si>
-  <si>
-    <t>-15.9908902645106</t>
-  </si>
-  <si>
-    <t>-47.9358386993394</t>
-  </si>
-  <si>
-    <t>-15.783298015594</t>
-  </si>
-  <si>
-    <t>-48.1016635894761</t>
-  </si>
-  <si>
-    <t>-15.9196507930751</t>
-  </si>
-  <si>
-    <t>-48.0925440788255</t>
-  </si>
-  <si>
-    <t>-15.8210635185237</t>
-  </si>
-  <si>
-    <t>-47.3735404014574</t>
-  </si>
-  <si>
-    <t>-15.7040226459499</t>
-  </si>
-  <si>
-    <t>-47.7632975578294</t>
-  </si>
-  <si>
-    <t>-15.7402324676509</t>
-  </si>
-  <si>
-    <t>-48.067417144774</t>
-  </si>
-  <si>
-    <t>-16.0136997699733</t>
-  </si>
-  <si>
-    <t>-47.8716588020311</t>
-  </si>
-  <si>
-    <t>-15.6003499031062</t>
-  </si>
-  <si>
-    <t>-47.9514169692979</t>
-  </si>
-  <si>
-    <t>-15.8500099182124</t>
-  </si>
-  <si>
-    <t>-47.9396367073045</t>
-  </si>
-  <si>
-    <t>-15.9336304664607</t>
-  </si>
-  <si>
-    <t>-47.7819657325731</t>
-  </si>
-  <si>
-    <t>-15.6504642963405</t>
-  </si>
-  <si>
-    <t>-47.9096817970262</t>
-  </si>
-  <si>
-    <t>-15.8326828479762</t>
-  </si>
-  <si>
-    <t>-48.0741977691636</t>
-  </si>
-  <si>
-    <t>-16.0116505622859</t>
-  </si>
-  <si>
-    <t>-47.6482844352708</t>
-  </si>
-  <si>
-    <t>-15.6028389930721</t>
-  </si>
-  <si>
-    <t>-48.0870294570909</t>
-  </si>
-  <si>
-    <t>-15.88415980339</t>
-  </si>
-  <si>
-    <t>-48.0997538566575</t>
-  </si>
-  <si>
-    <t>-15.9644651412959</t>
-  </si>
-  <si>
-    <t>-48.0024218559251</t>
-  </si>
-  <si>
-    <t>-16.0103952884669</t>
-  </si>
-  <si>
-    <t>-47.5556516647325</t>
-  </si>
-  <si>
-    <t>-16.0085391998286</t>
-  </si>
-  <si>
-    <t>-47.3805141448961</t>
-  </si>
-  <si>
-    <t>-16.016532182693</t>
-  </si>
-  <si>
-    <t>-47.9972720146165</t>
-  </si>
-  <si>
-    <t>-15.7834482192989</t>
-  </si>
-  <si>
-    <t>-48.0630397796617</t>
-  </si>
-  <si>
-    <t>-15.8364593982692</t>
-  </si>
-  <si>
-    <t>-48.059670925139</t>
-  </si>
-  <si>
-    <t>-15.795539617538</t>
-  </si>
-  <si>
-    <t>-47.9864573478685</t>
-  </si>
-  <si>
-    <t>-15.8183705806728</t>
-  </si>
-  <si>
-    <t>-47.8892111778245</t>
-  </si>
-  <si>
-    <t>-15.6459367275233</t>
-  </si>
-  <si>
-    <t>-47.9881095886217</t>
-  </si>
-  <si>
-    <t>-15.9931969642635</t>
-  </si>
-  <si>
-    <t>-47.6515674591051</t>
-  </si>
-  <si>
-    <t>-15.6247580051418</t>
-  </si>
-  <si>
-    <t>-48.0149316787706</t>
-  </si>
-  <si>
-    <t>-15.9475350379939</t>
-  </si>
-  <si>
-    <t>-47.6802349090562</t>
-  </si>
-  <si>
-    <t>-15.6201660633083</t>
-  </si>
-  <si>
-    <t>-47.793123722075</t>
-  </si>
-  <si>
-    <t>-15.876585245132</t>
-  </si>
-  <si>
-    <t>-47.9135441780076</t>
-  </si>
-  <si>
-    <t>-15.7087004184718</t>
-  </si>
-  <si>
-    <t>-48.0458307266221</t>
-  </si>
-  <si>
-    <t>-15.905767679214</t>
-  </si>
-  <si>
-    <t>-47.5213623046861</t>
-  </si>
-  <si>
-    <t>-15.6333196163173</t>
-  </si>
-  <si>
-    <t>-48.1365966796861</t>
-  </si>
-  <si>
-    <t>-15.7851541042323</t>
-  </si>
-  <si>
-    <t>-48.1686115264879</t>
-  </si>
-  <si>
-    <t>-15.5390453338619</t>
-  </si>
-  <si>
-    <t>-48.0721378326402</t>
-  </si>
-  <si>
-    <t>-15.980322360992</t>
-  </si>
-  <si>
-    <t>-47.9656219482408</t>
-  </si>
-  <si>
-    <t>-15.8703088760371</t>
-  </si>
-  <si>
-    <t>-48.0675458908067</t>
-  </si>
-  <si>
-    <t>-15.8229839801784</t>
-  </si>
-  <si>
-    <t>-47.8480339050279</t>
-  </si>
-  <si>
-    <t>-15.7951962947841</t>
-  </si>
-  <si>
-    <t>-48.2544851303087</t>
-  </si>
-  <si>
-    <t>-16.0436546802516</t>
-  </si>
-  <si>
-    <t>-48.1253743171678</t>
-  </si>
-  <si>
-    <t>-15.967179536819</t>
-  </si>
-  <si>
-    <t>-48.049221038817</t>
-  </si>
-  <si>
-    <t>-15.9094369411464</t>
-  </si>
-  <si>
-    <t>-47.8094744682298</t>
-  </si>
-  <si>
-    <t>-15.6548202037807</t>
-  </si>
-  <si>
-    <t>-47.8243660926805</t>
-  </si>
-  <si>
-    <t>-15.6446492671962</t>
-  </si>
-  <si>
-    <t>-48.0939602851854</t>
-  </si>
-  <si>
-    <t>-15.8012902736659</t>
-  </si>
-  <si>
-    <t>-48.0437493324266</t>
-  </si>
-  <si>
-    <t>-15.9012722969051</t>
-  </si>
-  <si>
-    <t>-48.0437922477708</t>
-  </si>
-  <si>
-    <t>-15.9227192401881</t>
-  </si>
-  <si>
-    <t>-48.0677175521837</t>
-  </si>
-  <si>
-    <t>-16.0134530067439</t>
-  </si>
-  <si>
-    <t>-48.142154216765</t>
-  </si>
-  <si>
-    <t>-15.890103578567</t>
-  </si>
-  <si>
-    <t>-48.0263257026658</t>
-  </si>
-  <si>
-    <t>-16.027153730392</t>
-  </si>
-  <si>
-    <t>-47.9421901702867</t>
-  </si>
-  <si>
-    <t>-15.8008074760432</t>
-  </si>
-  <si>
-    <t>-47.8549861907945</t>
-  </si>
-  <si>
-    <t>-15.846877098083</t>
-  </si>
-  <si>
-    <t>-48.1980943679796</t>
-  </si>
-  <si>
-    <t>-15.6651949882503</t>
-  </si>
-  <si>
-    <t>-48.1298375129686</t>
-  </si>
-  <si>
-    <t>-15.8069336414333</t>
-  </si>
-  <si>
-    <t>-47.618780136107</t>
-  </si>
-  <si>
-    <t>-15.5236172676082</t>
-  </si>
-  <si>
-    <t>-47.7717304229722</t>
-  </si>
-  <si>
-    <t>-15.916571617126</t>
-  </si>
-  <si>
-    <t>-47.7611732482896</t>
-  </si>
-  <si>
-    <t>-15.8979463577266</t>
-  </si>
-  <si>
-    <t>-47.7880382537828</t>
-  </si>
-  <si>
-    <t>-15.8955860137935</t>
-  </si>
-  <si>
-    <t>-47.7558517456041</t>
-  </si>
-  <si>
-    <t>-15.9051239490504</t>
-  </si>
-  <si>
-    <t>-48.0239224433885</t>
-  </si>
-  <si>
-    <t>-15.8856081962581</t>
-  </si>
-  <si>
-    <t>-48.0239868164049</t>
-  </si>
-  <si>
-    <t>-15.8595371246333</t>
-  </si>
-  <si>
-    <t>-48.0566239356981</t>
-  </si>
-  <si>
-    <t>-16.0253727436061</t>
-  </si>
-  <si>
-    <t>-47.6578116416917</t>
-  </si>
-  <si>
-    <t>-15.6149840354915</t>
-  </si>
-  <si>
-    <t>-47.9895901679979</t>
-  </si>
-  <si>
-    <t>-16.0073912143703</t>
-  </si>
-  <si>
-    <t>-48.1309747695909</t>
-  </si>
-  <si>
-    <t>-15.7956469058986</t>
-  </si>
-  <si>
-    <t>-48.0963635444627</t>
-  </si>
-  <si>
-    <t>-15.8309447765346</t>
-  </si>
-  <si>
-    <t>-47.7785968780504</t>
-  </si>
-  <si>
-    <t>-15.7706701755519</t>
-  </si>
-  <si>
-    <t>-48.200690746306</t>
-  </si>
-  <si>
-    <t>-15.6698405742641</t>
-  </si>
-  <si>
-    <t>-47.8468751907335</t>
-  </si>
-  <si>
-    <t>-15.6358623504634</t>
-  </si>
-  <si>
-    <t>-48.1121778488145</t>
-  </si>
-  <si>
-    <t>-15.8906614780421</t>
-  </si>
-  <si>
-    <t>-48.0734467506395</t>
-  </si>
-  <si>
-    <t>-16.0115647315974</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>-15.800896</t>
-  </si>
-  <si>
-    <t>-15.813201</t>
-  </si>
-  <si>
-    <t>-15.735378</t>
-  </si>
-  <si>
-    <t>-15.828578</t>
-  </si>
-  <si>
-    <t>-15.735693</t>
-  </si>
-  <si>
-    <t>-15.845447</t>
-  </si>
-  <si>
-    <t>-15.675074</t>
-  </si>
-  <si>
-    <t>-15.798894</t>
-  </si>
-  <si>
-    <t>-15.827313</t>
-  </si>
-  <si>
-    <t>-15.841474</t>
-  </si>
-  <si>
-    <t>-15.821942</t>
-  </si>
-  <si>
-    <t>-15.785673</t>
-  </si>
-  <si>
-    <t>-15.815309</t>
-  </si>
-  <si>
-    <t>-15.859855</t>
-  </si>
-  <si>
-    <t>-15.772759</t>
-  </si>
-  <si>
-    <t>-15.814717</t>
-  </si>
-  <si>
-    <t>-15.648612</t>
-  </si>
-  <si>
-    <t>-15.801392</t>
-  </si>
-  <si>
-    <t>-15.820160</t>
-  </si>
-  <si>
-    <t>-15.759256</t>
-  </si>
-  <si>
-    <t>-15.885181</t>
-  </si>
-  <si>
-    <t>-15.833847</t>
-  </si>
-  <si>
-    <t>-15.760302</t>
-  </si>
-  <si>
-    <t>-15.759768</t>
-  </si>
-  <si>
-    <t>-15.823967</t>
-  </si>
-  <si>
-    <t>-15.870194</t>
-  </si>
-  <si>
-    <t>-15.905819</t>
-  </si>
-  <si>
-    <t>-15.817710</t>
-  </si>
-  <si>
-    <t>-15.911784</t>
-  </si>
-  <si>
-    <t>-15.900793</t>
-  </si>
-  <si>
-    <t>-15.883017</t>
-  </si>
-  <si>
-    <t>-15.875977</t>
-  </si>
-  <si>
-    <t>-47.982235</t>
-  </si>
-  <si>
-    <t>-48.099695</t>
-  </si>
-  <si>
-    <t>-47.777748</t>
-  </si>
-  <si>
-    <t>-48.057594</t>
-  </si>
-  <si>
-    <t>-47.986099</t>
-  </si>
-  <si>
-    <t>-48.046297</t>
-  </si>
-  <si>
-    <t>-48.023552</t>
-  </si>
-  <si>
-    <t>-47.965691</t>
-  </si>
-  <si>
-    <t>-47.888969</t>
-  </si>
-  <si>
-    <t>-47.912131</t>
-  </si>
-  <si>
-    <t>-47.895309</t>
-  </si>
-  <si>
-    <t>-47.929166</t>
-  </si>
-  <si>
-    <t>-47.897239</t>
-  </si>
-  <si>
-    <t>-47.882990</t>
-  </si>
-  <si>
-    <t>-48.203996</t>
-  </si>
-  <si>
-    <t>-47.890001</t>
-  </si>
-  <si>
-    <t>-47.930522</t>
-  </si>
-  <si>
-    <t>-47.885285</t>
-  </si>
-  <si>
-    <t>-47.896106</t>
-  </si>
-  <si>
-    <t>-47.882863</t>
-  </si>
-  <si>
-    <t>-47.908292</t>
-  </si>
-  <si>
-    <t>-48.042606</t>
-  </si>
-  <si>
-    <t>-47.930484</t>
-  </si>
-  <si>
-    <t>-47.914739</t>
-  </si>
-  <si>
-    <t>-47.792290</t>
-  </si>
-  <si>
-    <t>-47.936691</t>
-  </si>
-  <si>
-    <t>-47.926535</t>
-  </si>
-  <si>
-    <t>-47.911386</t>
-  </si>
-  <si>
-    <t>-47.876796</t>
-  </si>
-  <si>
-    <t>-47.915299</t>
-  </si>
-  <si>
-    <t>-47.917464</t>
-  </si>
-  <si>
-    <t>-48.066628</t>
+    <t>Setor de Grandes Areas Sul 915</t>
+  </si>
+  <si>
+    <t>Area Especial 8, ae 8/9 sl 118 B</t>
+  </si>
+  <si>
+    <t>Area Especial – QI O6 Lote C – GuarA I</t>
+  </si>
+  <si>
+    <t>Quadra 400/600 Area Especial</t>
+  </si>
+  <si>
+    <t>QS 107 Conjunto 4 Area Especial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DF-075, KM 180, Area Especial EPNB</t>
+  </si>
+  <si>
+    <t>Area Especial 03, 3ª Avenida - NUcleo Bandeirante</t>
+  </si>
+  <si>
+    <t>Area Especial nº 6, Setor tradicional - Brazlandia</t>
   </si>
 </sst>
 </file>
@@ -2014,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D2" sqref="B2:D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,13 +2024,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="C1" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2047,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -2064,10 +2061,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2081,10 +2078,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -2098,10 +2095,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -2115,10 +2112,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -2132,10 +2129,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -2149,10 +2146,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -2166,10 +2163,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2183,10 +2180,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -2200,10 +2197,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -2217,10 +2214,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -2234,10 +2231,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -2251,10 +2248,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -2268,10 +2265,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
@@ -2285,10 +2282,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="D16" t="s">
         <v>29</v>
@@ -2302,10 +2299,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -2319,10 +2316,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2336,10 +2333,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -2353,10 +2350,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -2370,10 +2367,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
@@ -2387,10 +2384,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D22" t="s">
         <v>40</v>
@@ -2404,10 +2401,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -2421,10 +2418,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>
@@ -2438,10 +2435,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
@@ -2455,10 +2452,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
@@ -2472,10 +2469,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="D27" t="s">
         <v>49</v>
@@ -2486,10 +2483,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="D28" t="s">
         <v>50</v>
@@ -2503,10 +2500,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="D29" t="s">
         <v>52</v>
@@ -2520,10 +2517,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="D30" t="s">
         <v>53</v>
@@ -2537,10 +2534,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -2554,10 +2551,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
         <v>55</v>
@@ -2571,10 +2568,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -2588,10 +2585,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="D34" t="s">
         <v>57</v>
@@ -2605,10 +2602,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="D35" t="s">
         <v>59</v>
@@ -2622,10 +2619,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="D36" t="s">
         <v>61</v>
@@ -2639,10 +2636,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
@@ -2656,10 +2653,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="D38" t="s">
         <v>64</v>
@@ -2673,10 +2670,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="D39" t="s">
         <v>65</v>
@@ -2690,10 +2687,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D40" t="s">
         <v>67</v>
@@ -2707,10 +2704,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="D41" t="s">
         <v>68</v>
@@ -2724,10 +2721,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="D42" t="s">
         <v>69</v>
@@ -2741,10 +2738,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
@@ -2758,10 +2755,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="D44" t="s">
         <v>73</v>
@@ -2775,10 +2772,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="D45" t="s">
         <v>75</v>
@@ -2792,10 +2789,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="D46" t="s">
         <v>76</v>
@@ -2809,10 +2806,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="D47" t="s">
         <v>77</v>
@@ -2826,10 +2823,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="D48" t="s">
         <v>78</v>
@@ -2843,10 +2840,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="D49" t="s">
         <v>80</v>
@@ -2860,10 +2857,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="D50" t="s">
         <v>82</v>
@@ -2877,10 +2874,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="D51" t="s">
         <v>83</v>
@@ -2894,10 +2891,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="D52" t="s">
         <v>84</v>
@@ -2911,10 +2908,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="D53" t="s">
         <v>86</v>
@@ -2928,10 +2925,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="D54" t="s">
         <v>87</v>
@@ -2945,10 +2942,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="D55" t="s">
         <v>88</v>
@@ -2962,10 +2959,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="D56" t="s">
         <v>89</v>
@@ -2979,10 +2976,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="D57" t="s">
         <v>91</v>
@@ -2996,10 +2993,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="D58" t="s">
         <v>93</v>
@@ -3013,10 +3010,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="D59" t="s">
         <v>19</v>
@@ -3030,10 +3027,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="D60" t="s">
         <v>96</v>
@@ -3047,10 +3044,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -3064,10 +3061,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="D62" t="s">
         <v>98</v>
@@ -3081,10 +3078,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="D63" t="s">
         <v>100</v>
@@ -3098,10 +3095,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="D64" t="s">
         <v>102</v>
@@ -3115,10 +3112,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="D65" t="s">
         <v>103</v>
@@ -3132,10 +3129,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D66" t="s">
         <v>105</v>
@@ -3149,10 +3146,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D67" t="s">
         <v>106</v>
@@ -3166,10 +3163,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="D68" t="s">
         <v>108</v>
@@ -3183,10 +3180,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="D69" t="s">
         <v>110</v>
@@ -3200,10 +3197,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="D70" t="s">
         <v>111</v>
@@ -3217,10 +3214,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="D71" t="s">
         <v>112</v>
@@ -3234,10 +3231,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="D72" t="s">
         <v>114</v>
@@ -3251,10 +3248,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="D73" t="s">
         <v>115</v>
@@ -3268,10 +3265,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="D74" t="s">
         <v>116</v>
@@ -3285,10 +3282,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="D75" t="s">
         <v>117</v>
@@ -3302,10 +3299,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="D76" t="s">
         <v>118</v>
@@ -3319,10 +3316,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="D77" t="s">
         <v>120</v>
@@ -3336,10 +3333,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="D78" t="s">
         <v>121</v>
@@ -3353,10 +3350,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="D79" t="s">
         <v>122</v>
@@ -3370,10 +3367,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D80" t="s">
         <v>124</v>
@@ -3387,10 +3384,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="D81" t="s">
         <v>126</v>
@@ -3404,10 +3401,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D82" t="s">
         <v>128</v>
@@ -3421,10 +3418,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D83" t="s">
         <v>129</v>
@@ -3438,10 +3435,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D84" t="s">
         <v>130</v>
@@ -3455,10 +3452,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D85" t="s">
         <v>131</v>
@@ -3472,10 +3469,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="D86" t="s">
         <v>132</v>
@@ -3489,10 +3486,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="D87" t="s">
         <v>134</v>
@@ -3506,10 +3503,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D88" t="s">
         <v>135</v>
@@ -3523,10 +3520,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="D89" t="s">
         <v>136</v>
@@ -3540,10 +3537,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
@@ -3557,10 +3554,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="D91" t="s">
         <v>139</v>
@@ -3574,10 +3571,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D92" t="s">
         <v>128</v>
@@ -3591,10 +3588,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D93" t="s">
         <v>141</v>
@@ -3608,10 +3605,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="D94" t="s">
         <v>143</v>
@@ -3622,10 +3619,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D95" t="s">
         <v>144</v>
@@ -3639,10 +3636,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D96" t="s">
         <v>145</v>
@@ -3656,10 +3653,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="D97" t="s">
         <v>146</v>
@@ -3673,10 +3670,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="D98" t="s">
         <v>148</v>
@@ -3690,10 +3687,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="D99" t="s">
         <v>149</v>
@@ -3707,10 +3704,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="D100" t="s">
         <v>150</v>
@@ -3724,10 +3721,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="D101" t="s">
         <v>152</v>
@@ -3741,10 +3738,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="D102" t="s">
         <v>153</v>
@@ -3758,10 +3755,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D103" t="s">
         <v>155</v>
@@ -3775,10 +3772,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="D104" t="s">
         <v>157</v>
@@ -3792,10 +3789,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D105" t="s">
         <v>158</v>
@@ -3809,10 +3806,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D106" t="s">
         <v>159</v>
@@ -3826,10 +3823,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D107" t="s">
         <v>160</v>
@@ -3843,10 +3840,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="D108" t="s">
         <v>161</v>
@@ -3860,10 +3857,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="D109" t="s">
         <v>162</v>
@@ -3877,10 +3874,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="D110" t="s">
         <v>163</v>
@@ -3894,10 +3891,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D111" t="s">
         <v>165</v>
@@ -3911,10 +3908,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D112" t="s">
         <v>166</v>
@@ -3928,10 +3925,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D113" t="s">
         <v>167</v>
@@ -3945,10 +3942,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D114" t="s">
         <v>169</v>
@@ -3962,10 +3959,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D115" t="s">
         <v>170</v>
@@ -3979,10 +3976,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D116" t="s">
         <v>172</v>
@@ -3996,10 +3993,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="D117" t="s">
         <v>174</v>
@@ -4013,10 +4010,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="D118" t="s">
         <v>175</v>
@@ -4030,10 +4027,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D119" t="s">
         <v>176</v>
@@ -4047,10 +4044,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="D120" t="s">
         <v>177</v>
@@ -4064,10 +4061,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="D121" t="s">
         <v>179</v>
@@ -4081,10 +4078,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D122" t="s">
         <v>180</v>
@@ -4098,10 +4095,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D123" t="s">
         <v>181</v>
@@ -4115,10 +4112,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D124" t="s">
         <v>182</v>
@@ -4132,10 +4129,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D125" t="s">
         <v>183</v>
@@ -4149,10 +4146,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D126" t="s">
         <v>184</v>
@@ -4166,10 +4163,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="D127" t="s">
         <v>186</v>
@@ -4183,10 +4180,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D128" t="s">
         <v>187</v>
@@ -4200,10 +4197,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D129" t="s">
         <v>188</v>
@@ -4217,10 +4214,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D130" t="s">
         <v>128</v>
@@ -4234,10 +4231,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D131" t="s">
         <v>190</v>
@@ -4251,10 +4248,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D132" t="s">
         <v>191</v>
@@ -4268,10 +4265,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D133" t="s">
         <v>192</v>
@@ -4285,10 +4282,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="D134" t="s">
         <v>193</v>
@@ -4299,10 +4296,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="D135" t="s">
         <v>194</v>
@@ -4313,10 +4310,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="D136" t="s">
         <v>195</v>
@@ -4327,10 +4324,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="D137" t="s">
         <v>196</v>
@@ -4341,10 +4338,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="D138" t="s">
         <v>197</v>
@@ -4355,13 +4352,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="D139" t="s">
-        <v>198</v>
+        <v>538</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4369,13 +4366,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="D140" t="s">
-        <v>199</v>
+        <v>549</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4383,13 +4380,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="D141" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4397,13 +4394,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="D142" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4411,13 +4408,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="D143" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4425,13 +4422,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="D144" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4439,13 +4436,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="D145" t="s">
-        <v>204</v>
+        <v>539</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4453,13 +4450,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="D146" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4467,13 +4464,13 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C147" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D147" t="s">
         <v>540</v>
-      </c>
-      <c r="D147" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4481,13 +4478,13 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="D148" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4495,13 +4492,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="D149" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4509,13 +4506,13 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>209</v>
+        <v>541</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4523,13 +4520,13 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="D151" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4537,13 +4534,13 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="D152" t="s">
-        <v>211</v>
+        <v>542</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,13 +4548,13 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="D153" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4565,13 +4562,13 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="D154" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4579,13 +4576,13 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="D155" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4593,13 +4590,13 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="D156" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4607,13 +4604,13 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="D157" t="s">
-        <v>216</v>
+        <v>543</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4621,13 +4618,13 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="D158" t="s">
-        <v>217</v>
+        <v>548</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4635,13 +4632,13 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="D159" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4649,13 +4646,13 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="D160" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4663,13 +4660,13 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="D161" t="s">
-        <v>220</v>
+        <v>544</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4677,13 +4674,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D162" t="s">
-        <v>221</v>
+        <v>545</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4691,13 +4688,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="D163" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4705,13 +4702,13 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="D164" t="s">
-        <v>223</v>
+        <v>546</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,13 +4716,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="D165" t="s">
-        <v>224</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>